<commit_message>
Add sentences to spreadsheet.  Add text size option buttons to GUI
</commit_message>
<xml_diff>
--- a/worksheets/forms.xlsx
+++ b/worksheets/forms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-Q1R9F2N\Documents\Hobbies\Projects\Flash Cards\NT Greek FC\NT Greek FC\worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-Q1R9F2N\Documents\Hobbies\Projects\Flash Cards\NT Greek FC\worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D515806-0C16-49FB-8B1F-E954D7E48E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE562D2-E8E5-499D-96F0-6CE5F7AD0BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>nominative</t>
   </si>
   <si>
-    <t>acusative</t>
-  </si>
-  <si>
     <t>with</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>word</t>
+  </si>
+  <si>
+    <t>accusative</t>
   </si>
 </sst>
 </file>
@@ -156,21 +156,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +452,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,26 +462,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="4"/>
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
@@ -495,20 +492,19 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
       <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -516,20 +512,19 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5"/>
       <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -537,55 +532,53 @@
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
       <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="F9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="F9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="4"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
@@ -597,69 +590,65 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="6"/>
-      <c r="F16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="4"/>
       <c r="F17" s="1" t="s">
         <v>14</v>
       </c>
@@ -671,69 +660,65 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="E18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="E20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="F23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="6"/>
-      <c r="F23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="4"/>
       <c r="F24" s="1" t="s">
         <v>14</v>
       </c>
@@ -745,69 +730,65 @@
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="E25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="E26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="E27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="F31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="6"/>
-      <c r="F31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="6"/>
+      <c r="D32" s="4"/>
       <c r="F32" s="1" t="s">
         <v>14</v>
       </c>
@@ -819,69 +800,65 @@
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
       <c r="E33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="E34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="E35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
+      <c r="F39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="6"/>
-      <c r="F39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G39" s="3"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="6"/>
+      <c r="D40" s="4"/>
       <c r="F40" s="1" t="s">
         <v>14</v>
       </c>
@@ -893,62 +870,59 @@
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
       <c r="E41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
       <c r="E42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
       <c r="E43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>